<commit_message>
Joined figures code to analysis code. Updated plant growth form and elevation data for characters. Update units and README accordingly
</commit_message>
<xml_diff>
--- a/GUMOTTC_Data/gumottc_units.xlsx
+++ b/GUMOTTC_Data/gumottc_units.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="137">
   <si>
     <t>column_letter</t>
   </si>
@@ -264,13 +264,22 @@
     <t>Y</t>
   </si>
   <si>
+    <t>elevation_estimate</t>
+  </si>
+  <si>
+    <t>if elevation had to be estimated using coordinates determined via WGS84</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
     <t>match_below_500ft</t>
   </si>
   <si>
     <t>if sample has a species match in the other time period that was collected within 500ft of each other in terms of elevation</t>
   </si>
   <si>
-    <t>Z</t>
+    <t>AA</t>
   </si>
   <si>
     <t>match_500ft_id</t>
@@ -458,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -467,6 +476,12 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
@@ -1129,27 +1144,27 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="D26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1159,6 +1174,23 @@
         <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1207,7 +1239,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1221,16 +1253,16 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4">
@@ -1238,16 +1270,16 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5">
@@ -1255,10 +1287,10 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -1272,10 +1304,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -1289,16 +1321,16 @@
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
@@ -1306,16 +1338,16 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
@@ -1323,10 +1355,10 @@
         <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -1340,16 +1372,16 @@
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
@@ -1357,10 +1389,10 @@
         <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
@@ -1374,10 +1406,10 @@
         <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
@@ -1391,16 +1423,16 @@
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14">
@@ -1408,16 +1440,16 @@
         <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15">
@@ -1425,10 +1457,10 @@
         <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>8</v>
@@ -1482,7 +1514,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1547,16 +1579,16 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7">
@@ -1564,16 +1596,16 @@
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
@@ -1581,16 +1613,16 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
@@ -1598,84 +1630,84 @@
         <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>121</v>
+      <c r="B10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>122</v>
+      <c r="E10" s="6" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>123</v>
+      <c r="B11" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>125</v>
+      <c r="E11" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>126</v>
+      <c r="B12" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>122</v>
+      <c r="E12" s="6" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>127</v>
+      <c r="B13" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="14">
@@ -1683,33 +1715,33 @@
         <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>133</v>
+      <c r="B15" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>122</v>
+      <c r="E15" s="6" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>